<commit_message>
PC increment after indexed instruction
</commit_message>
<xml_diff>
--- a/Ramses/Project_tb/Set of instructions and registers output.xlsx
+++ b/Ramses/Project_tb/Set of instructions and registers output.xlsx
@@ -170,11 +170,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -455,15 +456,18 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I30"/>
+  <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+      <selection activeCell="J3" sqref="J3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="7" max="7" width="17.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B1" t="s">
         <v>16</v>
       </c>
@@ -477,7 +481,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B2" t="s">
         <v>21</v>
       </c>
@@ -502,8 +506,11 @@
       <c r="I2">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J2">
+        <v>4090</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>22</v>
       </c>
@@ -529,7 +536,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>24</v>
       </c>
@@ -549,7 +556,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>0</v>
       </c>
@@ -578,7 +585,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>1</v>
       </c>
@@ -601,7 +608,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>2</v>
       </c>
@@ -624,7 +631,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>3</v>
       </c>
@@ -647,7 +654,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>4</v>
       </c>
@@ -670,7 +677,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>5</v>
       </c>
@@ -693,7 +700,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
@@ -716,7 +723,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>7</v>
       </c>
@@ -739,7 +746,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>8</v>
       </c>
@@ -762,7 +769,7 @@
         <v>72</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>9</v>
       </c>
@@ -785,7 +792,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>10</v>
       </c>
@@ -808,7 +815,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>11</v>
       </c>
@@ -946,6 +953,9 @@
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>51</v>
+      </c>
+      <c r="G24" s="2">
+        <v>1001000110100</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Synthesis to be succesful
Modification con files to make synthesis succesful
</commit_message>
<xml_diff>
--- a/Ramses/Project_tb/Set of instructions and registers output.xlsx
+++ b/Ramses/Project_tb/Set of instructions and registers output.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="43" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="46" uniqueCount="40">
   <si>
     <t>R0</t>
   </si>
@@ -135,6 +135,15 @@
   </si>
   <si>
     <t>Second Indexed</t>
+  </si>
+  <si>
+    <t>Indirect</t>
+  </si>
+  <si>
+    <t>Move to address R14 (52) data in R8 (72)</t>
+  </si>
+  <si>
+    <t>4DE8</t>
   </si>
 </sst>
 </file>
@@ -459,7 +468,7 @@
   <dimension ref="A1:J30"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J3" sqref="J3"/>
+      <selection activeCell="J2" sqref="J2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -506,8 +515,8 @@
       <c r="I2">
         <v>2</v>
       </c>
-      <c r="J2">
-        <v>4090</v>
+      <c r="J2" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
@@ -535,6 +544,9 @@
       <c r="I3" t="s">
         <v>36</v>
       </c>
+      <c r="J3" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
@@ -607,6 +619,9 @@
       <c r="G6">
         <v>0</v>
       </c>
+      <c r="J6">
+        <v>0</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
@@ -630,6 +645,9 @@
       <c r="G7">
         <v>0</v>
       </c>
+      <c r="J7">
+        <v>0</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
@@ -653,6 +671,9 @@
       <c r="G8">
         <v>0</v>
       </c>
+      <c r="J8">
+        <v>0</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
@@ -676,6 +697,9 @@
       <c r="G9">
         <v>20</v>
       </c>
+      <c r="J9">
+        <v>20</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
@@ -699,6 +723,9 @@
       <c r="G10">
         <v>35</v>
       </c>
+      <c r="J10">
+        <v>35</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
@@ -722,6 +749,9 @@
       <c r="G11">
         <v>41</v>
       </c>
+      <c r="J11">
+        <v>41</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
@@ -745,6 +775,9 @@
       <c r="G12">
         <v>55</v>
       </c>
+      <c r="J12">
+        <v>55</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
@@ -768,6 +801,9 @@
       <c r="G13">
         <v>72</v>
       </c>
+      <c r="J13">
+        <v>72</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
@@ -791,6 +827,9 @@
       <c r="G14">
         <v>50</v>
       </c>
+      <c r="J14">
+        <v>50</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
@@ -814,6 +853,9 @@
       <c r="G15">
         <v>51</v>
       </c>
+      <c r="J15">
+        <v>51</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
@@ -837,8 +879,11 @@
       <c r="G16">
         <v>422</v>
       </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J16">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>12</v>
       </c>
@@ -860,8 +905,11 @@
       <c r="G17">
         <v>874</v>
       </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>874</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>13</v>
       </c>
@@ -883,8 +931,11 @@
       <c r="G18">
         <v>52</v>
       </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>14</v>
       </c>
@@ -906,8 +957,11 @@
       <c r="G19">
         <v>53</v>
       </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J19">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -929,8 +983,11 @@
       <c r="G20">
         <v>-4</v>
       </c>
-    </row>
-    <row r="22" spans="1:7" s="1" customFormat="1" ht="60" x14ac:dyDescent="0.25">
+      <c r="J20">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" s="1" customFormat="1" ht="75" x14ac:dyDescent="0.25">
       <c r="B22" s="1" t="s">
         <v>20</v>
       </c>
@@ -949,8 +1006,11 @@
       <c r="G22" s="1" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="J22" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>51</v>
       </c>
@@ -958,27 +1018,27 @@
         <v>1001000110100</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>52</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>53</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>54</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>55</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>56</v>
       </c>
@@ -986,7 +1046,7 @@
         <v>2345</v>
       </c>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>57</v>
       </c>

</xml_diff>